<commit_message>
fixed and added the test case headers
</commit_message>
<xml_diff>
--- a/homework2/Water_Dispenser_Traceability_matrix_Ivan_Voronkov.xlsx
+++ b/homework2/Water_Dispenser_Traceability_matrix_Ivan_Voronkov.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="Traceability matrix" sheetId="2" r:id="rId2"/>
+    <sheet name="Traceability matrix" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>Requirements</t>
   </si>
@@ -76,15 +76,9 @@
     <t>The water dispenser should have a lighting, which will allow pouring water in the dark. The end light must be controlled by the button.</t>
   </si>
   <si>
-    <t>The water dispenser should have a cooling mode of water, in which the water temperature should not exceed 12°C. The water dispenser mode must be controlled by a separate button.</t>
-  </si>
-  <si>
     <t>The water dispenser should be operated indoors at a positive temperature.</t>
   </si>
   <si>
-    <t>Test Scenarios</t>
-  </si>
-  <si>
     <t>R10</t>
   </si>
   <si>
@@ -115,27 +109,6 @@
     <t>R09</t>
   </si>
   <si>
-    <t>The water dispenser is unpacked in a room with a positive temperature and set it on the floor. Let's try to sway him. If it staggers, turn its leveling feet.</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>We take a bottle of water and put it on top of the water dispenser. Make sure that it does not fall out.</t>
-  </si>
-  <si>
-    <t>The power cord insert into the socket. We choose the energy-saving mode on the control panel. After 6 minutes, we draw water into the glass from the hot water outlet. We measure the temperature of the water in the glass.</t>
-  </si>
-  <si>
-    <t>Turn on the water cooling mode. When the "Cold" indicator goes off, we draw water into the glass from the cold water outlet. We measure the temperature of the water in the glass. We draw water into an empty glass from the hot water outlet and measure the temperature of the water.</t>
-  </si>
-  <si>
-    <t>We turn on the lighting mode with the "LIGHT ON/OFF" button. We re-press the "LIGHT ON/OFF" button to turn off the lighting mode.</t>
-  </si>
-  <si>
-    <t>There should not be break between 3 and 4 scenarios. Turn off the energy-saving mode. After 4 minutes, we draw water into the glass from the hot water outlet. We measure the temperature of the water in the glass.</t>
-  </si>
-  <si>
     <t>+
 It is precisely described how to install the water dispenser.</t>
   </si>
@@ -269,6 +242,42 @@
   <si>
     <t>+
 It is possible to write a test scenario.</t>
+  </si>
+  <si>
+    <t>Test case headers</t>
+  </si>
+  <si>
+    <t>Check the possibility of installation on the floor.</t>
+  </si>
+  <si>
+    <t>Check the possibility of installing a water bottle on the water intake.</t>
+  </si>
+  <si>
+    <t>Check the possibility of switching the water heating modes with a single button.</t>
+  </si>
+  <si>
+    <t>Measure the water temperature from the hot water outlet after 6 minutes after switching on.</t>
+  </si>
+  <si>
+    <t>Measure the water temperature from the hot water outlet after 10 minutes after switching on.</t>
+  </si>
+  <si>
+    <t>Measure the water temperature from the cold water outlet.</t>
+  </si>
+  <si>
+    <t>The water dispenser should have a cooling mode of water, in which the water temperature should not exceed 12°C.</t>
+  </si>
+  <si>
+    <t>Make sure that hot and cold water flows from different outlets.</t>
+  </si>
+  <si>
+    <t>Check for lighting.</t>
+  </si>
+  <si>
+    <t>Check for leveling feet for floor installation.</t>
+  </si>
+  <si>
+    <t>Check the possibility of using the water dispenser indoors with a positive temperature.</t>
   </si>
 </sst>
 </file>
@@ -301,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -550,11 +559,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,45 +615,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -653,6 +642,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1011,7 +1015,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1031,26 +1035,26 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>37</v>
+      <c r="C2" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>11</v>
@@ -1063,20 +1067,20 @@
       <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>38</v>
+      <c r="C3" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>11</v>
@@ -1086,23 +1090,23 @@
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>40</v>
+      <c r="C4" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>11</v>
@@ -1115,20 +1119,20 @@
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>40</v>
+      <c r="C5" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>11</v>
@@ -1138,49 +1142,49 @@
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>41</v>
+      <c r="C6" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>66</v>
+      <c r="B7" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="G7" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1193,20 +1197,20 @@
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>64</v>
+      <c r="C8" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>11</v>
@@ -1219,20 +1223,20 @@
       <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="28" t="s">
-        <v>65</v>
+      <c r="C9" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>11</v>
@@ -1243,22 +1247,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>39</v>
+        <v>17</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>11</v>
@@ -1268,23 +1272,23 @@
       <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>43</v>
+      <c r="B11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>11</v>
@@ -1298,184 +1302,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="60.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="B2" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B5" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B6" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B7" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B8" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B9" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
-        <v>1</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="15"/>
-    </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
-    </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="17"/>
+      <c r="B10" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>